<commit_message>
working on tests for updated warnings in fromwexcel.py
</commit_message>
<xml_diff>
--- a/test/data/cldf/defective_dataset/empty_excel.xlsx
+++ b/test/data/cldf/defective_dataset/empty_excel.xlsx
@@ -13,36 +13,17 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>walter.fuchs</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Language comment</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
+  <si>
+    <t>asdfasdf</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,19 +33,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,13 +57,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -390,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D1" sqref="D1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -401,15 +368,33 @@
     <col min="4" max="4" width="93.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>